<commit_message>
add new farewell sheet
</commit_message>
<xml_diff>
--- a/farewell_data.xlsx
+++ b/farewell_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>Timestamp</t>
   </si>
@@ -372,6 +372,48 @@
   </si>
   <si>
     <t>You have to stop think that what other thinks and do things the way you like.your a pure hearted person .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivek </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhaiya are the most motivating player . Player ke bad 
+Senior adviser ki post aapke ke best h mujhe ek bar aapki captaincy me khelna tha vo *sml* me khle liya.😁
+Bhaiya bike thodi slow chlaya kro 😅
+Day one pe lga ki bhai sab ke kon h in bhaiya ne to bhout attitude h bde gusse vale h  but gradually you are like big brother 🙃
+Best wishes for you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aapki captaincy me volleyball iitgn  ne phla tournament jita spoke summit or inter IIT me bhi aapn pre quarters  me pahuche 
+Or ha bhaiya mere bhout jyada bolne ka hisab game me pura ho gya tha na  🙃😁
+Bhaiya aapka time to time kudasan jana 😁😅
+</t>
+  </si>
+  <si>
+    <t>Bhaiya aapki calmness ka me fan ho gya jab bhi tatu , abhinav bhaiya over aggression me hote the you were the the middle men 
+Aapke sath intelectual bate krne me bde mje aate the . Aapki set ki hue ball le taappe marne me bde mje aate the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garu bhaiya 🙃😅  aapka har bat pr salah dena .
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Didi jab aapse phli abt mila to me dr dya tha aap is time pr abhinav  bhaiya me gussa kr rhe the   
+Then I was like iitne gusse vale senior then uske bad kabhi aapka gussa nhi dekha mene 
+Aapka bar bar. Muje ye bolna ki bibek muje hote bhadani h kya kr hu 😆
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Didi you are like the don 😆😅  aapka vo thada sa guise vala fce usme aap bhout funny lgte ho 🙂
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are the most cutest senior 🙃😅 
+Aapki serve ke bde charche h volleyball samj </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I found you as the most serious senior among all maine aajoo jyada mjak masti krte huee nhi Deka h .
+Aapke bina aaki team </t>
   </si>
 </sst>
 </file>
@@ -535,10 +577,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -546,13 +588,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -666,7 +708,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L11" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L12" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="12">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Name" id="2"/>
@@ -1240,20 +1282,52 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13">
+      <c r="A11" s="7">
         <v>45767.76726270834</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="8" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="13">
+        <v>45767.84058173611</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>